<commit_message>
Corrigidos DS + Adicionada descrição de CobrarRenda
</commit_message>
<xml_diff>
--- a/Fase 2/F2-Especificação_UC.xlsx
+++ b/Fase 2/F2-Especificação_UC.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UM\Informática\3º Ano\1º Semestre\DSS\dss-1617\Fase 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win8\Documents\GitHub\dss-1617\Fase 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="23040" windowHeight="8808" tabRatio="856" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="23040" windowHeight="8808" tabRatio="856" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Adicionar Despesa Extraord." sheetId="9" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="Alterar Renda do Apartamento" sheetId="6" r:id="rId5"/>
     <sheet name="Autenticar Utilizador" sheetId="11" r:id="rId6"/>
     <sheet name="Carregar Conta" sheetId="5" r:id="rId7"/>
-    <sheet name="Pagar Despesa" sheetId="10" r:id="rId8"/>
-    <sheet name="Regista Apartamento" sheetId="7" r:id="rId9"/>
-    <sheet name="Remover Morador" sheetId="3" r:id="rId10"/>
-    <sheet name="Ver Despesas Pagas" sheetId="13" r:id="rId11"/>
-    <sheet name="Ver Despesas por Pagar" sheetId="12" r:id="rId12"/>
+    <sheet name="Cobrar Renda" sheetId="14" r:id="rId8"/>
+    <sheet name="Pagar Despesa" sheetId="10" r:id="rId9"/>
+    <sheet name="Regista Apartamento" sheetId="7" r:id="rId10"/>
+    <sheet name="Remover Morador" sheetId="3" r:id="rId11"/>
+    <sheet name="Ver Despesas Pagas" sheetId="13" r:id="rId12"/>
+    <sheet name="Ver Despesas por Pagar" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="131">
   <si>
     <r>
       <t xml:space="preserve">  </t>
@@ -463,6 +464,34 @@
   <si>
     <t>Excepção 3               (passo 7)
 [dados do apartamento inválidos]</t>
+  </si>
+  <si>
+    <t>Cobrar Renda</t>
+  </si>
+  <si>
+    <t>Senhorio indica que quer cobrar renda</t>
+  </si>
+  <si>
+    <t>Adicionar a renda à lista das despesas por pagar de todos os moradores de um apartamento</t>
+  </si>
+  <si>
+    <t>Informa que a renda foi cobrada</t>
+  </si>
+  <si>
+    <t>Indica que não existem moradores registados no apartamento</t>
+  </si>
+  <si>
+    <t>Excepção 1               (passo 3)
+[não existem moradores]</t>
+  </si>
+  <si>
+    <t>Verifica, para cada morador, se a renda já foi cobrada este mês</t>
+  </si>
+  <si>
+    <t>Calcula renda total de cada morador cuja renda ainda não foi cobrada</t>
+  </si>
+  <si>
+    <t>Adiciona renda total à lista das despesas por pagar de cada morador cuja renda ainda não foi cobrada</t>
   </si>
 </sst>
 </file>
@@ -963,16 +992,16 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.83984375" style="4"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
     <col min="3" max="3" width="39" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.62890625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="1"/>
+    <col min="4" max="4" width="41.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>6</v>
       </c>
@@ -986,7 +1015,7 @@
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>0</v>
       </c>
@@ -1000,7 +1029,7 @@
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>1</v>
       </c>
@@ -1014,7 +1043,7 @@
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>2</v>
       </c>
@@ -1026,7 +1055,7 @@
       <c r="G6" s="26"/>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="28"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28" t="s">
@@ -1040,7 +1069,7 @@
       <c r="G7" s="27"/>
       <c r="H7" s="27"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>3</v>
       </c>
@@ -1056,7 +1085,7 @@
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="26"/>
       <c r="B9" s="29">
         <v>2</v>
@@ -1070,7 +1099,7 @@
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="26"/>
       <c r="B10" s="29">
         <v>3</v>
@@ -1084,7 +1113,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="26"/>
       <c r="B11" s="29">
         <v>4</v>
@@ -1098,7 +1127,7 @@
       <c r="G11" s="26"/>
       <c r="H11" s="26"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
       <c r="B12" s="29">
         <v>5</v>
@@ -1112,7 +1141,7 @@
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="32"/>
       <c r="B13" s="28"/>
       <c r="C13" s="28" t="s">
@@ -1126,7 +1155,7 @@
       <c r="G13" s="26"/>
       <c r="H13" s="26"/>
     </row>
-    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
         <v>108</v>
       </c>
@@ -1142,7 +1171,7 @@
       <c r="G14" s="26"/>
       <c r="H14" s="34"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="29">
         <v>2</v>
@@ -1156,7 +1185,7 @@
       <c r="G15" s="26"/>
       <c r="H15" s="26"/>
     </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L17" s="33"/>
     </row>
   </sheetData>
@@ -1167,57 +1196,51 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J18"/>
+  <dimension ref="A3:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.15625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83984375" style="4"/>
-    <col min="3" max="3" width="48" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.83984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="18.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="46.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1225,92 +1248,172 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D8" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="4">
+        <f>1+B8</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="29">
+        <f t="shared" ref="B10:B16" si="0">1+B9</f>
         <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="4">
-        <v>4</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="29">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="29">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="4">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="29">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="29">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="7"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="29">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="D15" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="5"/>
-      <c r="B16" s="4">
-        <v>2</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="29">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="6"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="32"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="29">
+        <v>1</v>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="D18" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="32"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="29">
+        <v>1</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="31"/>
+      <c r="B21" s="29">
+        <v>2</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
+      <c r="B28" s="4">
+        <v>2</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>120</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1320,60 +1423,65 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I13"/>
+  <dimension ref="A3:J18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.15625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83984375" style="4"/>
-    <col min="3" max="3" width="40.26171875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.62890625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="48" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1381,40 +1489,84 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>2</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>3</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="5"/>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>4</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="6"/>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="4">
+        <v>5</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="4">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="4">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1424,22 +1576,126 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:I13"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="40.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="4">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.15625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83984375" style="4"/>
-    <col min="3" max="3" width="40.26171875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.26171875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="40.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1447,7 +1703,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1455,7 +1711,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1463,12 +1719,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1476,7 +1732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1487,7 +1743,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -1495,7 +1751,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -1503,7 +1759,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="4">
         <v>4</v>
@@ -1512,11 +1768,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="8"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
     </row>
   </sheetData>
@@ -1533,16 +1789,16 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.83984375" style="4"/>
-    <col min="3" max="3" width="36.15625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.62890625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="36.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>6</v>
       </c>
@@ -1556,7 +1812,7 @@
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>0</v>
       </c>
@@ -1570,7 +1826,7 @@
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>1</v>
       </c>
@@ -1584,7 +1840,7 @@
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>2</v>
       </c>
@@ -1596,7 +1852,7 @@
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="18" t="s">
@@ -1610,7 +1866,7 @@
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
@@ -1626,7 +1882,7 @@
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="19">
         <v>2</v>
@@ -1640,7 +1896,7 @@
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="19">
         <v>3</v>
@@ -1654,7 +1910,7 @@
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="19">
         <v>4</v>
@@ -1668,7 +1924,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
       <c r="B12" s="19">
         <v>5</v>
@@ -1682,7 +1938,7 @@
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18" t="s">
@@ -1696,7 +1952,7 @@
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
     </row>
-    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>108</v>
       </c>
@@ -1712,7 +1968,7 @@
       <c r="G14" s="16"/>
       <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
       <c r="B15" s="19">
         <v>2</v>
@@ -1726,7 +1982,7 @@
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
     </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L17" s="23"/>
     </row>
   </sheetData>
@@ -1743,16 +1999,16 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.15625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.83984375" style="4"/>
-    <col min="3" max="3" width="46.68359375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.26171875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="20.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="46.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1760,7 +2016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1768,7 +2024,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1776,7 +2032,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1784,7 +2040,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -1794,7 +2050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1806,7 +2062,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -1814,7 +2070,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -1822,7 +2078,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="4">
         <v>4</v>
@@ -1832,7 +2088,7 @@
       </c>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>5</v>
       </c>
@@ -1840,7 +2096,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>6</v>
       </c>
@@ -1848,7 +2104,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>7</v>
       </c>
@@ -1856,7 +2112,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>8</v>
       </c>
@@ -1864,7 +2120,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>9</v>
       </c>
@@ -1872,7 +2128,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
@@ -1882,7 +2138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>13</v>
       </c>
@@ -1894,7 +2150,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>2</v>
       </c>
@@ -1902,7 +2158,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
@@ -1912,7 +2168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>15</v>
       </c>
@@ -1924,7 +2180,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
         <v>2</v>
       </c>
@@ -1932,22 +2188,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
     </row>
-    <row r="33" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
     </row>
   </sheetData>
@@ -1964,16 +2220,16 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.15625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.83984375" style="4"/>
-    <col min="3" max="3" width="44.26171875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="15.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="44.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1981,7 +2237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1989,7 +2245,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1997,12 +2253,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -2012,7 +2268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -2023,7 +2279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -2031,7 +2287,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -2039,7 +2295,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>4</v>
       </c>
@@ -2047,7 +2303,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>5</v>
       </c>
@@ -2055,7 +2311,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>6</v>
       </c>
@@ -2063,7 +2319,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -2073,7 +2329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
@@ -2085,7 +2341,7 @@
       </c>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>2</v>
       </c>
@@ -2093,7 +2349,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
@@ -2103,7 +2359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>34</v>
       </c>
@@ -2114,7 +2370,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>2</v>
       </c>
@@ -2122,7 +2378,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G21" s="9"/>
     </row>
   </sheetData>
@@ -2136,18 +2392,18 @@
   <dimension ref="A3:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.15625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.83984375" style="4"/>
-    <col min="3" max="4" width="43.83984375" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="15.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="4" width="43.88671875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2155,7 +2411,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -2163,7 +2419,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -2171,12 +2427,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
@@ -2184,7 +2440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -2195,7 +2451,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -2203,7 +2459,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="4">
         <v>3</v>
@@ -2212,7 +2468,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="4">
         <v>4</v>
@@ -2221,10 +2477,10 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
@@ -2235,7 +2491,7 @@
       </c>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
@@ -2246,7 +2502,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="4">
         <v>2</v>
@@ -2256,13 +2512,13 @@
       </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
     </row>
   </sheetData>
@@ -2279,16 +2535,16 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.15625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83984375" style="4"/>
-    <col min="3" max="3" width="34.83984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="34.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2296,7 +2552,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -2304,17 +2560,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -2322,7 +2578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -2333,7 +2589,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -2341,7 +2597,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -2349,10 +2605,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="C12" s="3" t="s">
         <v>4</v>
@@ -2361,7 +2617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>63</v>
       </c>
@@ -2372,7 +2628,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>2</v>
       </c>
@@ -2394,16 +2650,16 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.15625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83984375" style="4"/>
-    <col min="3" max="3" width="35.41796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.68359375" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="35.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2411,7 +2667,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -2419,7 +2675,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -2427,12 +2683,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -2440,7 +2696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -2451,7 +2707,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -2459,7 +2715,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -2467,7 +2723,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="4">
         <v>4</v>
@@ -2476,7 +2732,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="4">
         <v>5</v>
@@ -2485,15 +2741,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
     </row>
   </sheetData>
@@ -2504,22 +2760,205 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="77.21875" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="85.33203125" style="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="29"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="29"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="29"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="29"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="29">
+        <v>1</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="29"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="29"/>
+      <c r="B9" s="29">
+        <v>2</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="29">
+        <v>3</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="29">
+        <v>4</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
+      <c r="B12" s="29">
+        <v>5</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="32"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" s="29">
+        <v>1</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="31"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="31"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="31"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="31"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83984375" style="1"/>
-    <col min="3" max="3" width="48.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="48.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
@@ -2536,7 +2975,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
@@ -2553,7 +2992,7 @@
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -2570,7 +3009,7 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -2585,7 +3024,7 @@
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="14" t="s">
@@ -2602,7 +3041,7 @@
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -2621,7 +3060,7 @@
       <c r="J8" s="11"/>
       <c r="K8" s="15"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="12">
         <v>2</v>
@@ -2638,7 +3077,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="12">
         <v>3</v>
@@ -2655,7 +3094,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="12">
         <v>4</v>
@@ -2672,7 +3111,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="12">
         <v>5</v>
@@ -2689,7 +3128,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="12">
         <v>6</v>
@@ -2706,7 +3145,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="12">
         <v>7</v>
@@ -2723,7 +3162,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="12">
         <v>8</v>
@@ -2740,7 +3179,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="14" t="s">
@@ -2757,7 +3196,7 @@
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
     </row>
-    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>88</v>
       </c>
@@ -2767,233 +3206,6 @@
       <c r="C17" s="11"/>
       <c r="D17" s="12" t="s">
         <v>106</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="18.62890625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.83984375" style="4"/>
-    <col min="3" max="3" width="46.3125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.68359375" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="4">
-        <f>1+B8</f>
-        <v>2</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="29">
-        <f t="shared" ref="B10:B16" si="0">1+B9</f>
-        <v>3</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="29">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="29">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="29">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="29">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="29">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="29">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="32"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18" s="29">
-        <v>1</v>
-      </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="32"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="B20" s="29">
-        <v>1</v>
-      </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="31"/>
-      <c r="B21" s="29">
-        <v>2</v>
-      </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="7"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="6"/>
-      <c r="B28" s="4">
-        <v>2</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionado Diagrama de UC para CobrarRenda (e alterada especificação) + Adicionados comentários às classes Morador e Quarto
</commit_message>
<xml_diff>
--- a/Fase 2/F2-Especificação_UC.xlsx
+++ b/Fase 2/F2-Especificação_UC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="23040" windowHeight="8808" tabRatio="856" firstSheet="4" activeTab="7"/>
+    <workbookView minimized="1" xWindow="0" yWindow="456" windowWidth="23040" windowHeight="8808" tabRatio="856" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Adicionar Despesa Extraord." sheetId="9" r:id="rId1"/>
@@ -988,7 +988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -2763,7 +2763,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Adicionado cobrar renda aos textos dos use case e coluna do tipo de despesa
</commit_message>
<xml_diff>
--- a/Fase 2/F2-Especificação_UC.xlsx
+++ b/Fase 2/F2-Especificação_UC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win8\Documents\GitHub\dss-1617\Fase 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UM\Informática\3º Ano\1º Semestre\DSS\dss-1617\dss-1617\Fase 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -992,16 +992,16 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="19" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="8.89453125" style="4"/>
     <col min="3" max="3" width="39" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="41.68359375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="28" t="s">
         <v>6</v>
       </c>
@@ -1015,7 +1015,7 @@
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="29" t="s">
         <v>0</v>
       </c>
@@ -1029,7 +1029,7 @@
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="29" t="s">
         <v>1</v>
       </c>
@@ -1043,7 +1043,7 @@
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="29" t="s">
         <v>2</v>
       </c>
@@ -1055,7 +1055,7 @@
       <c r="G6" s="26"/>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="28"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28" t="s">
@@ -1069,7 +1069,7 @@
       <c r="G7" s="27"/>
       <c r="H7" s="27"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="29" t="s">
         <v>3</v>
       </c>
@@ -1085,7 +1085,7 @@
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="26"/>
       <c r="B9" s="29">
         <v>2</v>
@@ -1099,7 +1099,7 @@
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="26"/>
       <c r="B10" s="29">
         <v>3</v>
@@ -1113,7 +1113,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="26"/>
       <c r="B11" s="29">
         <v>4</v>
@@ -1127,7 +1127,7 @@
       <c r="G11" s="26"/>
       <c r="H11" s="26"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="30"/>
       <c r="B12" s="29">
         <v>5</v>
@@ -1141,7 +1141,7 @@
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="32"/>
       <c r="B13" s="28"/>
       <c r="C13" s="28" t="s">
@@ -1155,7 +1155,7 @@
       <c r="G13" s="26"/>
       <c r="H13" s="26"/>
     </row>
-    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="31" t="s">
         <v>108</v>
       </c>
@@ -1171,7 +1171,7 @@
       <c r="G14" s="26"/>
       <c r="H14" s="34"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="31"/>
       <c r="B15" s="29">
         <v>2</v>
@@ -1185,7 +1185,7 @@
       <c r="G15" s="26"/>
       <c r="H15" s="26"/>
     </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="12:12" x14ac:dyDescent="0.55000000000000004">
       <c r="L17" s="33"/>
     </row>
   </sheetData>
@@ -1202,16 +1202,16 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
-    <col min="3" max="3" width="46.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="18.68359375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.89453125" style="4"/>
+    <col min="3" max="3" width="46.3125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.68359375" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1235,12 +1235,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4">
         <f>1+B8</f>
         <v>2</v>
@@ -1268,7 +1268,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="29">
         <f t="shared" ref="B10:B16" si="0">1+B9</f>
         <v>3</v>
@@ -1277,7 +1277,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="29">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1286,7 +1286,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="29">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1295,7 +1295,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="29">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1304,7 +1304,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="29">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1313,7 +1313,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="29">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1322,7 +1322,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="29">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1331,7 +1331,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="32"/>
       <c r="B17" s="28"/>
       <c r="C17" s="28" t="s">
@@ -1341,7 +1341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="31" t="s">
         <v>117</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="32"/>
       <c r="B19" s="28"/>
       <c r="C19" s="28" t="s">
@@ -1363,7 +1363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="31" t="s">
         <v>119</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="31"/>
       <c r="B21" s="29">
         <v>2</v>
@@ -1385,7 +1385,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="7"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
@@ -1395,7 +1395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="6" t="s">
         <v>121</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="6"/>
       <c r="B28" s="4">
         <v>2</v>
@@ -1429,16 +1429,16 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="15.1015625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.89453125" style="4"/>
     <col min="3" max="3" width="48" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="43.89453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -1481,7 +1481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="4">
         <v>4</v>
       </c>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="4">
         <v>5</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="4">
         <v>7</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -1543,7 +1543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
         <v>24</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5"/>
       <c r="B16" s="4">
         <v>2</v>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="J16" s="9"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6"/>
     </row>
   </sheetData>
@@ -1582,16 +1582,16 @@
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
-    <col min="3" max="3" width="40.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.1015625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.89453125" style="4"/>
+    <col min="3" max="3" width="40.20703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.68359375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1615,12 +1615,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5"/>
       <c r="B11" s="4">
         <v>4</v>
@@ -1666,10 +1666,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6"/>
     </row>
   </sheetData>
@@ -1686,16 +1686,16 @@
       <selection activeCell="A8" sqref="A8:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
-    <col min="3" max="3" width="40.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.1015625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.89453125" style="4"/>
+    <col min="3" max="3" width="40.20703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.20703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1719,12 +1719,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5"/>
       <c r="B11" s="4">
         <v>4</v>
@@ -1768,11 +1768,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5"/>
       <c r="B12" s="8"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6"/>
     </row>
   </sheetData>
@@ -1789,16 +1789,16 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="19" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
-    <col min="3" max="3" width="36.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="8.89453125" style="4"/>
+    <col min="3" max="3" width="36.1015625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.68359375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="18" t="s">
         <v>6</v>
       </c>
@@ -1812,7 +1812,7 @@
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="19" t="s">
         <v>0</v>
       </c>
@@ -1826,7 +1826,7 @@
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="19" t="s">
         <v>1</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="19" t="s">
         <v>2</v>
       </c>
@@ -1852,7 +1852,7 @@
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="18" t="s">
@@ -1866,7 +1866,7 @@
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
@@ -1882,7 +1882,7 @@
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="16"/>
       <c r="B9" s="19">
         <v>2</v>
@@ -1896,7 +1896,7 @@
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="16"/>
       <c r="B10" s="19">
         <v>3</v>
@@ -1910,7 +1910,7 @@
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="16"/>
       <c r="B11" s="19">
         <v>4</v>
@@ -1924,7 +1924,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="20"/>
       <c r="B12" s="19">
         <v>5</v>
@@ -1938,7 +1938,7 @@
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="22"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18" t="s">
@@ -1952,7 +1952,7 @@
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
     </row>
-    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="21" t="s">
         <v>108</v>
       </c>
@@ -1968,7 +1968,7 @@
       <c r="G14" s="16"/>
       <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="21"/>
       <c r="B15" s="19">
         <v>2</v>
@@ -1982,7 +1982,7 @@
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
     </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="12:12" x14ac:dyDescent="0.55000000000000004">
       <c r="L17" s="23"/>
     </row>
   </sheetData>
@@ -1999,16 +1999,16 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
-    <col min="3" max="3" width="46.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="20.1015625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.89453125" style="4"/>
+    <col min="3" max="3" width="46.68359375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.20703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -2050,7 +2050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -2062,7 +2062,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5"/>
       <c r="B11" s="4">
         <v>4</v>
@@ -2088,7 +2088,7 @@
       </c>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="4">
         <v>5</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="4">
         <v>6</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="4">
         <v>7</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="4">
         <v>8</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="4">
         <v>9</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
@@ -2138,7 +2138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
         <v>13</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="4">
         <v>2</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="7"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
@@ -2168,7 +2168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="6" t="s">
         <v>15</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="4">
         <v>2</v>
       </c>
@@ -2188,22 +2188,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="7"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="6"/>
     </row>
-    <row r="33" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="7"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="6"/>
     </row>
   </sheetData>
@@ -2220,16 +2220,16 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
-    <col min="3" max="3" width="44.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.1015625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.89453125" style="4"/>
+    <col min="3" max="3" width="44.20703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -2253,12 +2253,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -2268,7 +2268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="4">
         <v>4</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="4">
         <v>5</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="4">
         <v>6</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -2329,7 +2329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="4">
         <v>2</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
@@ -2359,7 +2359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
         <v>34</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="4">
         <v>2</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G21" s="9"/>
     </row>
   </sheetData>
@@ -2395,15 +2395,15 @@
       <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
-    <col min="3" max="4" width="43.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.1015625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.89453125" style="4"/>
+    <col min="3" max="4" width="43.89453125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -2427,12 +2427,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5"/>
       <c r="B10" s="4">
         <v>3</v>
@@ -2468,7 +2468,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5"/>
       <c r="B11" s="4">
         <v>4</v>
@@ -2477,10 +2477,10 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
@@ -2491,7 +2491,7 @@
       </c>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6"/>
       <c r="B15" s="4">
         <v>2</v>
@@ -2512,13 +2512,13 @@
       </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6"/>
     </row>
   </sheetData>
@@ -2535,16 +2535,16 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
-    <col min="3" max="3" width="34.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1015625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.89453125" style="4"/>
+    <col min="3" max="3" width="34.89453125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -2560,17 +2560,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -2605,10 +2605,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5"/>
       <c r="C12" s="3" t="s">
         <v>4</v>
@@ -2617,7 +2617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
         <v>63</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="4">
         <v>2</v>
       </c>
@@ -2650,16 +2650,16 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
-    <col min="3" max="3" width="35.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.1015625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.89453125" style="4"/>
+    <col min="3" max="3" width="35.41796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.68359375" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -2683,12 +2683,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5"/>
       <c r="B11" s="4">
         <v>4</v>
@@ -2732,7 +2732,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5"/>
       <c r="B12" s="4">
         <v>5</v>
@@ -2741,15 +2741,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6"/>
     </row>
   </sheetData>
@@ -2766,27 +2766,27 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" style="30" customWidth="1"/>
-    <col min="3" max="3" width="77.21875" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="85.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7890625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.41796875" style="30" customWidth="1"/>
+    <col min="3" max="3" width="73.68359375" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.20703125" style="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="29"/>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="29"/>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="28" t="s">
         <v>6</v>
       </c>
@@ -2796,7 +2796,7 @@
       </c>
       <c r="D3" s="29"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="29" t="s">
         <v>0</v>
       </c>
@@ -2806,7 +2806,7 @@
       </c>
       <c r="D4" s="29"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="29" t="s">
         <v>1</v>
       </c>
@@ -2816,7 +2816,7 @@
       </c>
       <c r="D5" s="29"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="29" t="s">
         <v>2</v>
       </c>
@@ -2824,7 +2824,7 @@
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="29"/>
       <c r="B7" s="29"/>
       <c r="C7" s="29" t="s">
@@ -2834,7 +2834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="29" t="s">
         <v>3</v>
       </c>
@@ -2846,7 +2846,7 @@
       </c>
       <c r="D8" s="29"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="29"/>
       <c r="B9" s="29">
         <v>2</v>
@@ -2856,7 +2856,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="29">
         <v>3</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="29">
         <v>4</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="30"/>
       <c r="B12" s="29">
         <v>5</v>
@@ -2884,13 +2884,13 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="29"/>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="32"/>
       <c r="B14" s="28"/>
       <c r="C14" s="28" t="s">
@@ -2900,7 +2900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="31" t="s">
         <v>127</v>
       </c>
@@ -2912,25 +2912,25 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="31"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
       <c r="D16" s="29"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="31"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
       <c r="D17" s="29"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="31"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="31"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
@@ -2949,16 +2949,16 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="48.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.1015625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.89453125" style="1"/>
+    <col min="3" max="3" width="48.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.5234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
@@ -2975,7 +2975,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
@@ -2992,7 +2992,7 @@
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -3009,7 +3009,7 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -3024,7 +3024,7 @@
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="14" t="s">
@@ -3041,7 +3041,7 @@
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -3060,7 +3060,7 @@
       <c r="J8" s="11"/>
       <c r="K8" s="15"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="11"/>
       <c r="B9" s="12">
         <v>2</v>
@@ -3077,7 +3077,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="11"/>
       <c r="B10" s="12">
         <v>3</v>
@@ -3094,7 +3094,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="11"/>
       <c r="B11" s="12">
         <v>4</v>
@@ -3111,7 +3111,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="11"/>
       <c r="B12" s="12">
         <v>5</v>
@@ -3128,7 +3128,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="11"/>
       <c r="B13" s="12">
         <v>6</v>
@@ -3145,7 +3145,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="11"/>
       <c r="B14" s="12">
         <v>7</v>
@@ -3162,7 +3162,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="11"/>
       <c r="B15" s="12">
         <v>8</v>
@@ -3179,7 +3179,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="14" t="s">
@@ -3196,7 +3196,7 @@
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
     </row>
-    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="13" t="s">
         <v>88</v>
       </c>

</xml_diff>